<commit_message>
relatorio finalizado. adicionado esquema global.
</commit_message>
<xml_diff>
--- a/Relatório Projecto Final/Schemas/Modelo EA.xlsx
+++ b/Relatório Projecto Final/Schemas/Modelo EA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
-  <si>
-    <t>Notificações</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>ContentProvider</t>
   </si>
   <si>
     <t>Thoth</t>
-  </si>
-  <si>
-    <t>Notification</t>
   </si>
   <si>
     <t>Loader</t>
@@ -64,6 +58,21 @@
   </si>
   <si>
     <t>IselAppReceiver</t>
+  </si>
+  <si>
+    <t>IselAppSyncAdapter</t>
+  </si>
+  <si>
+    <t>CalendarEvents</t>
+  </si>
+  <si>
+    <t>NotificationLaunch</t>
+  </si>
+  <si>
+    <t>Calendar Provider</t>
+  </si>
+  <si>
+    <t>Notifications</t>
   </si>
 </sst>
 </file>
@@ -353,6 +362,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -383,9 +395,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,13 +416,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
@@ -454,16 +463,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>29415</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>144462</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>192087</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -480,7 +489,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6448425" y="2714625"/>
+          <a:off x="9525000" y="3914775"/>
           <a:ext cx="896190" cy="725487"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -492,13 +501,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -539,13 +548,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>240631</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>155407</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>345907</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>55144</xdr:rowOff>
@@ -593,28 +602,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>256048</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>41929</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:rowOff>2708</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>50131</xdr:rowOff>
+      <xdr:rowOff>10910</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="9" name="Straight Connector 8"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="7" idx="3"/>
-        </xdr:cNvCxnSpPr>
+        <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3925680" y="2378061"/>
-          <a:ext cx="355557" cy="8202"/>
+          <a:off x="6973974" y="3678237"/>
+          <a:ext cx="354673" cy="8202"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -639,13 +646,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>155407</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>155407</xdr:rowOff>
@@ -683,13 +690,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -727,13 +734,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>185487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>5013</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -774,13 +781,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>280736</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>185487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>281115</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>158595</xdr:rowOff>
@@ -821,13 +828,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -865,13 +872,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>280736</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>5013</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>5013</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>5013</xdr:rowOff>
@@ -909,13 +916,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>245644</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
@@ -953,13 +960,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>240631</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>240631</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>50132</xdr:rowOff>
@@ -997,13 +1004,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>240631</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>55145</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>55145</xdr:rowOff>
@@ -1044,13 +1051,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>606592</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1091,13 +1098,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>13939</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>604024</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
@@ -1139,13 +1146,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>604344</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>6571</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -1187,13 +1194,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>611605</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>355934</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>80210</xdr:rowOff>
@@ -1212,6 +1219,475 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Connector 19"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4267200" y="3857625"/>
+          <a:ext cx="0" cy="590550"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>605088</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>185988</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Arrow Connector 25"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4257675" y="4438650"/>
+          <a:ext cx="3053013" cy="5013"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Connector 27"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7924800" y="4057650"/>
+          <a:ext cx="0" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>502</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Connector 29"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6981825" y="4057650"/>
+          <a:ext cx="943477" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>290513</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>63598</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>290892</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Straight Arrow Connector 31"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6996113" y="3730723"/>
+          <a:ext cx="379" cy="331690"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>10583</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>10584</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Straight Arrow Connector 34"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7979833" y="4667250"/>
+          <a:ext cx="10584" cy="370417"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9491</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>10584</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>529166</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>175462</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Straight Arrow Connector 36"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8624324" y="3100917"/>
+          <a:ext cx="1133509" cy="1339628"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>253999</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>611784</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>8202</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Straight Connector 39"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9482666" y="5238750"/>
+          <a:ext cx="357785" cy="8202"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>145677</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>145677</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>250953</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>45414</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="Oval 40"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9334501" y="5199530"/>
+          <a:ext cx="105276" cy="90237"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-PT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>184899</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>145677</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>296</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Straight Arrow Connector 41"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="41" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8578103" y="5238752"/>
+          <a:ext cx="756398" cy="5897"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
@@ -2677,99 +3153,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G9:T20"/>
+  <dimension ref="A9:N28"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="9.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="9" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K9" s="33" t="s">
+    <row r="9" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E9" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="23"/>
+    </row>
+    <row r="10" spans="5:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+    </row>
+    <row r="11" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G11" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="25"/>
+      <c r="J11" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="25"/>
+    </row>
+    <row r="12" spans="5:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="26"/>
+      <c r="H12" s="27"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="27"/>
+    </row>
+    <row r="14" spans="5:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="G15" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="25"/>
+      <c r="J15" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="29"/>
+      <c r="L15" s="30"/>
+    </row>
+    <row r="16" spans="5:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="26"/>
+      <c r="H16" s="27"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="33"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="D19" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="25"/>
+      <c r="G19" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="L9" s="33"/>
-    </row>
-    <row r="10" spans="11:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-    </row>
-    <row r="11" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="M11" s="23" t="s">
+      <c r="H19" s="25"/>
+      <c r="M19" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" s="25"/>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="26"/>
+      <c r="B20" s="27"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="27"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="27"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G23" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="30"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G24" s="31"/>
+      <c r="H24" s="33"/>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G27" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="N11" s="24"/>
-      <c r="P11" s="23" t="s">
-        <v>3</v>
+      <c r="H27" s="30"/>
+      <c r="K27" s="28" t="s">
+        <v>14</v>
       </c>
-      <c r="Q11" s="24"/>
-    </row>
-    <row r="12" spans="11:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M12" s="25"/>
-      <c r="N12" s="26"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="26"/>
-    </row>
-    <row r="14" spans="11:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="M15" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="N15" s="24"/>
-      <c r="P15" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="29"/>
-    </row>
-    <row r="16" spans="11:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M16" s="25"/>
-      <c r="N16" s="26"/>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="32"/>
-    </row>
-    <row r="18" spans="7:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G19" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" s="24"/>
-      <c r="J19" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="K19" s="24"/>
-      <c r="M19" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="N19" s="24"/>
-      <c r="S19" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="T19" s="24"/>
-    </row>
-    <row r="20" spans="7:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G20" s="25"/>
-      <c r="H20" s="26"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="26"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="26"/>
-      <c r="S20" s="25"/>
-      <c r="T20" s="26"/>
+      <c r="L27" s="30"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="31"/>
+      <c r="H28" s="33"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="M15:N16"/>
+  <mergeCells count="12">
+    <mergeCell ref="A19:B20"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="G23:H24"/>
+    <mergeCell ref="G27:H28"/>
+    <mergeCell ref="K27:L28"/>
+    <mergeCell ref="E9:F10"/>
+    <mergeCell ref="G15:H16"/>
+    <mergeCell ref="G19:H20"/>
     <mergeCell ref="M19:N20"/>
-    <mergeCell ref="S19:T20"/>
-    <mergeCell ref="P11:Q12"/>
-    <mergeCell ref="J19:K20"/>
-    <mergeCell ref="P15:R16"/>
-    <mergeCell ref="G19:H20"/>
-    <mergeCell ref="M11:N12"/>
+    <mergeCell ref="J11:K12"/>
+    <mergeCell ref="D19:E20"/>
+    <mergeCell ref="J15:L16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2781,7 +3291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
@@ -2816,19 +3326,19 @@
     </row>
     <row r="7" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="29"/>
+      <c r="H7" s="30"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="18"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="32"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="33"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
@@ -2883,14 +3393,14 @@
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C16" s="5"/>
-      <c r="D16" s="27" t="s">
-        <v>7</v>
+      <c r="D16" s="28" t="s">
+        <v>5</v>
       </c>
-      <c r="E16" s="29"/>
+      <c r="E16" s="30"/>
     </row>
     <row r="17" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="30"/>
-      <c r="E17" s="32"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="33"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
@@ -2940,18 +3450,18 @@
     <row r="25" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E25" s="20"/>
       <c r="F25" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
-      <c r="G25" s="27" t="s">
-        <v>9</v>
+      <c r="G25" s="28" t="s">
+        <v>7</v>
       </c>
-      <c r="H25" s="29"/>
+      <c r="H25" s="30"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
     </row>
     <row r="26" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G26" s="30"/>
-      <c r="H26" s="32"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="33"/>
       <c r="I26" s="6"/>
       <c r="J26" s="7"/>
     </row>

</xml_diff>